<commit_message>
added missing config to pretest self test question
</commit_message>
<xml_diff>
--- a/Templates/SubscriberMap.xlsx
+++ b/Templates/SubscriberMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="131">
   <si>
     <t>Id</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>B2603773-852F-11E7-BB31-BE2E44B06B34</t>
+  </si>
+  <si>
+    <t>clientSelfTestesd</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37:O38"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,8 +2084,12 @@
       <c r="D38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="G38" s="2" t="s">
         <v>18</v>
       </c>
@@ -2100,7 +2107,7 @@
       </c>
       <c r="O38" t="str">
         <f>Table1[[#This Row],[Id]]&amp;N38&amp;Table1[[#This Row],[Name]]&amp;N38&amp;Table1[[#This Row],[Field]]&amp;N38&amp;Table1[[#This Row],[Type]]&amp;N38&amp;Table1[[#This Row],[SubName]]&amp;N38&amp;Table1[[#This Row],[SubField]]&amp;N38&amp;Table1[[#This Row],[SubType]]&amp;N38&amp;Table1[[#This Row],[Group]]&amp;N38&amp;Table1[[#This Row],[Mode]]&amp;N38&amp;Table1[[#This Row],[SectionId]]&amp;N38&amp;Table1[[#This Row],[FormId]]&amp;N38&amp;Table1[[#This Row],[SubscriberSystemId]]</f>
-        <v>1a28a864-a84f-13e7-abc4-cec278b6b50a|Obs|B2603773-852F-11E7-BB31-BE2E44B06B34|Concept|||Single|5||||16E23866-9D69-11E7-ABC4-CEC278B6B50A</v>
+        <v>1a28a864-a84f-13e7-abc4-cec278b6b50a|Obs|B2603773-852F-11E7-BB31-BE2E44B06B34|Concept|DTL_FBCUSTOMFIELD_HTC_Lab_MOH_362|clientSelfTestesd|Single|5||||16E23866-9D69-11E7-ABC4-CEC278B6B50A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>